<commit_message>
Added JUnit driven by spreadsheet
</commit_message>
<xml_diff>
--- a/camunda/camunda-spring-boot-app/src/test/resources/Testcase-Example-2.xlsx
+++ b/camunda/camunda-spring-boot-app/src/test/resources/Testcase-Example-2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t xml:space="preserve">Workflow ID</t>
   </si>
@@ -67,6 +67,15 @@
     <t xml:space="preserve">Review1</t>
   </si>
   <si>
+    <t xml:space="preserve">Happy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">something</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FormError</t>
+  </si>
+  <si>
     <t xml:space="preserve">Approved</t>
   </si>
   <si>
@@ -77,6 +86,9 @@
   </si>
   <si>
     <t xml:space="preserve">Approved2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End</t>
   </si>
 </sst>
 </file>
@@ -92,6 +104,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -113,6 +126,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -157,7 +171,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -174,11 +188,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -199,15 +209,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="8:8"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.43"/>
@@ -224,101 +234,128 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="2" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="B5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="0" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="4" t="b">
+      <c r="B7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="4" t="b">
+      <c r="C8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="0" t="s">
+      <c r="C9" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3"/>
-      <c r="B10" s="5"/>
-    </row>
-    <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G11" s="3"/>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G13" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>